<commit_message>
Added a field in history route
</commit_message>
<xml_diff>
--- a/questionFile.xlsx
+++ b/questionFile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>question_body</t>
   </si>
@@ -35,15 +35,9 @@
     <t>is_exact_match</t>
   </si>
   <si>
-    <t>question1 daily</t>
-  </si>
-  <si>
     <t>abc</t>
   </si>
   <si>
-    <t>question2 daily</t>
-  </si>
-  <si>
     <t>question1 weekly</t>
   </si>
   <si>
@@ -54,6 +48,17 @@
   </si>
   <si>
     <t>question question</t>
+  </si>
+  <si>
+    <t>#MarkDown Question 1
+* point1
+``` Code code ```
+Answer - abc</t>
+  </si>
+  <si>
+    <t>#MarkDown Question 2
+``` Code code ```
+Answer - bcd</t>
   </si>
 </sst>
 </file>
@@ -89,8 +94,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -387,7 +395,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -399,15 +407,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -418,18 +426,18 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" t="b">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -437,7 +445,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -445,7 +453,35 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" t="b">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" t="b">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>